<commit_message>
added lesson: work with libraries docxtpl python-pptx XlsxWriter docx2pdf python-docx
</commit_message>
<xml_diff>
--- a/vgu/диаграммы.xlsx
+++ b/vgu/диаграммы.xlsx
@@ -61,14 +61,11 @@
   <c:chart>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!A1:A7</c:f>
@@ -100,40 +97,22 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:marker val="1"/>
-        <c:axId val="50010001"/>
-        <c:axId val="50010002"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50010001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50010002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>

</xml_diff>